<commit_message>
Updated Data Types of Drivers data file
</commit_message>
<xml_diff>
--- a/DB Types.xlsx
+++ b/DB Types.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SANA JALGAONKAR\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juyinshafaqinamdar/Documents/GitHub/Database-and-Analytical-Programming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A3E665-7FB0-4170-8D17-B0978AD048D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{051F680A-416F-7B41-B8BC-D6B77F164F56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1882C850-AB2B-4B0B-A79C-EC8EF5C50AE0}"/>
+    <workbookView xWindow="4660" yWindow="500" windowWidth="23260" windowHeight="12460" activeTab="1" xr2:uid="{1882C850-AB2B-4B0B-A79C-EC8EF5C50AE0}"/>
   </bookViews>
   <sheets>
     <sheet name="Incident data" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="96">
   <si>
     <t xml:space="preserve">id </t>
   </si>
@@ -194,6 +194,138 @@
   </si>
   <si>
     <t>latitude</t>
+  </si>
+  <si>
+    <t>Report Number</t>
+  </si>
+  <si>
+    <t>Local Case Number</t>
+  </si>
+  <si>
+    <t>Agency Name</t>
+  </si>
+  <si>
+    <t>ACRS Report Type</t>
+  </si>
+  <si>
+    <t>Crash Date/Time</t>
+  </si>
+  <si>
+    <t>Route Type</t>
+  </si>
+  <si>
+    <t>Road Name</t>
+  </si>
+  <si>
+    <t>Cross-Street Type</t>
+  </si>
+  <si>
+    <t>Cross-Street Name</t>
+  </si>
+  <si>
+    <t>Off-Road Description</t>
+  </si>
+  <si>
+    <t>Municipality</t>
+  </si>
+  <si>
+    <t>Related Non-Motorist</t>
+  </si>
+  <si>
+    <t>Collision Type</t>
+  </si>
+  <si>
+    <t>Weather</t>
+  </si>
+  <si>
+    <t>Surface Condition</t>
+  </si>
+  <si>
+    <t>Light</t>
+  </si>
+  <si>
+    <t>Traffic Control</t>
+  </si>
+  <si>
+    <t>Driver Substance Abuse</t>
+  </si>
+  <si>
+    <t>Non-Motorist Substance Abuse</t>
+  </si>
+  <si>
+    <t>Person ID</t>
+  </si>
+  <si>
+    <t>Driver At Fault</t>
+  </si>
+  <si>
+    <t>Injury Severity</t>
+  </si>
+  <si>
+    <t>Circumstance</t>
+  </si>
+  <si>
+    <t>Driver Distracted By</t>
+  </si>
+  <si>
+    <t>Drivers License State</t>
+  </si>
+  <si>
+    <t>Vehicle ID</t>
+  </si>
+  <si>
+    <t>Vehicle Damage Extent</t>
+  </si>
+  <si>
+    <t>Vehicle First Impact Location</t>
+  </si>
+  <si>
+    <t>Vehicle Second Impact Location</t>
+  </si>
+  <si>
+    <t>Vehicle Body Type</t>
+  </si>
+  <si>
+    <t>Vehicle Movement</t>
+  </si>
+  <si>
+    <t>Vehicle Continuing Dir</t>
+  </si>
+  <si>
+    <t>Vehicle Going Dir</t>
+  </si>
+  <si>
+    <t>Speed Limit</t>
+  </si>
+  <si>
+    <t>Driverless Vehicle</t>
+  </si>
+  <si>
+    <t>Parked Vehicle</t>
+  </si>
+  <si>
+    <t>Vehicle Year</t>
+  </si>
+  <si>
+    <t>Vehicle Make</t>
+  </si>
+  <si>
+    <t>Vehicle Model</t>
+  </si>
+  <si>
+    <t>Equipment Problems</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>DATE</t>
   </si>
 </sst>
 </file>
@@ -575,17 +707,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA0E614D-CCAC-45E6-BC74-B4C80223DBB6}">
   <dimension ref="A1:B44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.6640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -593,7 +725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -601,7 +733,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -609,7 +741,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -617,7 +749,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -625,7 +757,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -633,7 +765,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -641,7 +773,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -649,7 +781,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -657,7 +789,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
@@ -665,7 +797,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
@@ -673,7 +805,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
@@ -681,7 +813,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -689,7 +821,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
@@ -697,7 +829,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
@@ -705,7 +837,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
@@ -713,7 +845,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
@@ -721,7 +853,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
@@ -729,7 +861,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
@@ -737,7 +869,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>26</v>
       </c>
@@ -745,7 +877,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>27</v>
       </c>
@@ -753,7 +885,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>28</v>
       </c>
@@ -761,7 +893,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>29</v>
       </c>
@@ -769,7 +901,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>31</v>
       </c>
@@ -777,7 +909,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>32</v>
       </c>
@@ -785,7 +917,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>33</v>
       </c>
@@ -793,7 +925,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>34</v>
       </c>
@@ -801,7 +933,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>35</v>
       </c>
@@ -809,7 +941,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>36</v>
       </c>
@@ -817,7 +949,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>37</v>
       </c>
@@ -825,7 +957,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>38</v>
       </c>
@@ -833,7 +965,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>39</v>
       </c>
@@ -841,7 +973,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>40</v>
       </c>
@@ -849,7 +981,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>41</v>
       </c>
@@ -857,7 +989,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>42</v>
       </c>
@@ -865,7 +997,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>43</v>
       </c>
@@ -873,7 +1005,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>44</v>
       </c>
@@ -881,7 +1013,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>45</v>
       </c>
@@ -889,7 +1021,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>46</v>
       </c>
@@ -897,7 +1029,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>47</v>
       </c>
@@ -905,7 +1037,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>48</v>
       </c>
@@ -913,7 +1045,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>49</v>
       </c>
@@ -921,7 +1053,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>51</v>
       </c>
@@ -929,7 +1061,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>50</v>
       </c>
@@ -944,12 +1076,362 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4AC471D-5EB4-4A92-8C06-2F984C052FA6}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B43" sqref="A1:B43"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>75</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>76</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>80</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>81</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>82</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>83</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>84</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>85</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>86</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>87</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>88</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>89</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>90</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>91</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>92</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>93</v>
+      </c>
+      <c r="B42" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>94</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -960,7 +1442,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Data type for drivers in excel file
</commit_message>
<xml_diff>
--- a/DB Types.xlsx
+++ b/DB Types.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juyinshafaqinamdar/Documents/GitHub/Database-and-Analytical-Programming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{051F680A-416F-7B41-B8BC-D6B77F164F56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD68767-F5EB-5D4E-92DC-6151BB51A747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4660" yWindow="500" windowWidth="23260" windowHeight="12460" activeTab="1" xr2:uid="{1882C850-AB2B-4B0B-A79C-EC8EF5C50AE0}"/>
   </bookViews>
@@ -325,14 +325,14 @@
     <t>Location</t>
   </si>
   <si>
-    <t>DATE</t>
+    <t>DOUBLE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -344,6 +344,18 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -366,9 +378,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1078,20 +1092,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4AC471D-5EB4-4A92-8C06-2F984C052FA6}">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B43" sqref="A1:B43"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1099,7 +1114,7 @@
       <c r="A2" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1107,7 +1122,7 @@
       <c r="A3" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1115,7 +1130,7 @@
       <c r="A4" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1123,15 +1138,15 @@
       <c r="A5" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>95</v>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1139,7 +1154,7 @@
       <c r="A7" t="s">
         <v>58</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1147,7 +1162,7 @@
       <c r="A8" t="s">
         <v>59</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1155,7 +1170,7 @@
       <c r="A9" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1163,7 +1178,7 @@
       <c r="A10" t="s">
         <v>61</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1171,7 +1186,7 @@
       <c r="A11" t="s">
         <v>62</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1179,7 +1194,7 @@
       <c r="A12" t="s">
         <v>63</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1187,7 +1202,7 @@
       <c r="A13" t="s">
         <v>64</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1195,7 +1210,7 @@
       <c r="A14" t="s">
         <v>65</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1203,7 +1218,7 @@
       <c r="A15" t="s">
         <v>66</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1211,7 +1226,7 @@
       <c r="A16" t="s">
         <v>67</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1219,7 +1234,7 @@
       <c r="A17" t="s">
         <v>68</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1227,7 +1242,7 @@
       <c r="A18" t="s">
         <v>69</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1235,7 +1250,7 @@
       <c r="A19" t="s">
         <v>70</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1243,7 +1258,7 @@
       <c r="A20" t="s">
         <v>71</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1251,7 +1266,7 @@
       <c r="A21" t="s">
         <v>72</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1259,7 +1274,7 @@
       <c r="A22" t="s">
         <v>73</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1267,7 +1282,7 @@
       <c r="A23" t="s">
         <v>74</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1275,7 +1290,7 @@
       <c r="A24" t="s">
         <v>75</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1283,7 +1298,7 @@
       <c r="A25" t="s">
         <v>76</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1291,7 +1306,7 @@
       <c r="A26" t="s">
         <v>77</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1299,7 +1314,7 @@
       <c r="A27" t="s">
         <v>78</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1307,7 +1322,7 @@
       <c r="A28" t="s">
         <v>79</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1315,7 +1330,7 @@
       <c r="A29" t="s">
         <v>80</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1323,7 +1338,7 @@
       <c r="A30" t="s">
         <v>81</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1331,7 +1346,7 @@
       <c r="A31" t="s">
         <v>82</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1339,7 +1354,7 @@
       <c r="A32" t="s">
         <v>83</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1347,7 +1362,7 @@
       <c r="A33" t="s">
         <v>84</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1355,7 +1370,7 @@
       <c r="A34" t="s">
         <v>85</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1363,7 +1378,7 @@
       <c r="A35" t="s">
         <v>86</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1371,7 +1386,7 @@
       <c r="A36" t="s">
         <v>87</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1379,7 +1394,7 @@
       <c r="A37" t="s">
         <v>88</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1387,7 +1402,7 @@
       <c r="A38" t="s">
         <v>89</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1395,7 +1410,7 @@
       <c r="A39" t="s">
         <v>90</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1403,7 +1418,7 @@
       <c r="A40" t="s">
         <v>91</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1411,23 +1426,23 @@
       <c r="A41" t="s">
         <v>92</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>4</v>
+      <c r="B41" s="2" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>93</v>
       </c>
-      <c r="B42" t="s">
-        <v>18</v>
+      <c r="B42" s="3" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>94</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="2" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>